<commit_message>
add: graphic interface for wifi module.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="92">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,156 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WI-FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nochka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60 dbm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; dbm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,"-"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,'-'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-Z,a-z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~!@#$%^&amp;*()_=+?/&lt;&gt;,.|\{}[]`"':;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APs_SSID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APs_RSSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~`!@#$%^&amp;*()_-+={}[]:"|;'\&lt;&gt;?,./</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nkidjuesloik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WPA_WPA2_PSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdanab.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~`!@#$%^&amp;*()_-+={}[]:"|;'\&lt;&gt;?,./ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modalWindowTitle</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1604,9 @@
       </c>
       <c r="G6"/>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1471,6 +1623,29 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1488,6 +1663,29 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1503,6 +1701,27 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1520,6 +1739,29 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1601,6 +1843,227 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
refactor: web client and wifi scanning procedure.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="92">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1532,9 +1532,13 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1568,9 +1572,13 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>56</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1602,10 +1610,12 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1933,7 +1943,7 @@
         <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -1950,7 +1960,7 @@
         <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
add: uart top layer driver, logging, time support.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="94">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t xml:space="preserve">modalWindowTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital_clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;time&gt;</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1541,9 @@
       <c r="G4" t="s">
         <v>67</v>
       </c>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
       <c r="I4" t="s">
         <v>56</v>
       </c>
@@ -1727,9 +1735,7 @@
         <v>17</v>
       </c>
       <c r="G9"/>
-      <c r="H9" t="s">
-        <v>76</v>
-      </c>
+      <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="L9" s="11" t="s">
@@ -1974,24 +1980,24 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -2003,32 +2009,32 @@
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -2037,15 +2043,15 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -2054,15 +2060,15 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -2071,7 +2077,7 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>